<commit_message>
Added calculation of ullage level height
</commit_message>
<xml_diff>
--- a/Thick Walled PV Basic Stress Calc.xlsx
+++ b/Thick Walled PV Basic Stress Calc.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD Documents\Rocketry\Propulsion Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3B2D3D0B-6CEA-443A-A040-2786BFD5122D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{27AE3C5D-3511-4AB5-BAC9-F1852AB5542B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{838B0196-D158-479E-A7C6-911A07F6EFB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{838B0196-D158-479E-A7C6-911A07F6EFB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs + Answers" sheetId="1" r:id="rId1"/>
     <sheet name="Calcs" sheetId="2" r:id="rId2"/>
+    <sheet name="Bolt Calcs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Dan Zanko - 7/22/2018</t>
   </si>
@@ -238,12 +239,84 @@
   <si>
     <t>Inputs</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">THESE ARE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FINAL CALCS</t>
+    </r>
+  </si>
+  <si>
+    <t>Long. Stress (psi)</t>
+  </si>
+  <si>
+    <t>Inner End-cap Radius (in.)</t>
+  </si>
+  <si>
+    <t>Internal Surf. Area of End Cap (in^2)</t>
+  </si>
+  <si>
+    <t>Calcs are assuming perfectly hemispherical end caps</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">THESE ARE EQUATIONS I DERIVED ON MY OWN TO GET A QUICK ESTIMATE OF CLAMP FORCE REQD </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>due to longitudinal forces only</t>
+    </r>
+  </si>
+  <si>
+    <t>Longitudinal Force (lbf)</t>
+  </si>
+  <si>
+    <t>Number of Bolts (integer)</t>
+  </si>
+  <si>
+    <t>Nominal Bolt Diameter (in.)</t>
+  </si>
+  <si>
+    <t>Clamp Force Required per Bolt (lbf)</t>
+  </si>
+  <si>
+    <t>Tensile Stress on Each Bolt (psi)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +393,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -359,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -402,6 +501,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,49 +635,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7804.411764705882</c:v>
+                  <c:v>7002.6470588235297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7727.5902576552571</c:v>
+                  <c:v>6933.7175973059757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7652.7814893270324</c:v>
+                  <c:v>6866.5941013524525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7579.9157566996546</c:v>
+                  <c:v>6801.2140286889799</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7508.9263481849339</c:v>
+                  <c:v>6737.5175211582846</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7439.7493908806118</c:v>
+                  <c:v>6675.4472676644618</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7372.3237068455655</c:v>
+                  <c:v>6614.9483752133438</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7306.5906777936098</c:v>
+                  <c:v>6555.9682475066156</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7242.4941176470593</c:v>
+                  <c:v>6498.4564705882349</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7179.980152432533</c:v>
+                  <c:v>6442.3647050788086</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7118.9971070395377</c:v>
+                  <c:v>6387.6465845677158</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7059.4953983973128</c:v>
+                  <c:v>6334.2576197641456</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7001.4274346575257</c:v>
+                  <c:v>6282.1551080369709</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6944.7475200000008</c:v>
+                  <c:v>6231.2980480000006</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6889.411764705882</c:v>
+                  <c:v>6181.6470588235297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,46 +780,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-915</c:v>
+                  <c:v>-821</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-838.17849294937537</c:v>
+                  <c:v>-752.07053848244539</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-763.36972462115091</c:v>
+                  <c:v>-684.94704252892336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-690.50399199377262</c:v>
+                  <c:v>-619.56696986545069</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-619.51458347905157</c:v>
+                  <c:v>-555.87046233475519</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-550.33762617472996</c:v>
+                  <c:v>-493.80020884093233</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-482.91194213968339</c:v>
+                  <c:v>-433.30131638981402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-417.17891308772636</c:v>
+                  <c:v>-374.32118868308595</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-353.08235294117634</c:v>
+                  <c:v>-316.80941176470566</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-290.56838772665054</c:v>
+                  <c:v>-260.71764625527885</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-229.58534233365435</c:v>
+                  <c:v>-205.99952574418646</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-170.08363369143007</c:v>
+                  <c:v>-152.61056094061664</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-112.01566995164301</c:v>
+                  <c:v>-100.50804921344123</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-55.335755294118094</c:v>
+                  <c:v>-49.650989176470745</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -820,49 +925,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3444.705882352941</c:v>
+                  <c:v>3090.8235294117649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -971,49 +1076,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7551.2320942921951</c:v>
+                  <c:v>6775.477103184583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7418.1733409665039</c:v>
+                  <c:v>6656.0877736978155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7288.6007533703687</c:v>
+                  <c:v>6539.8264683246707</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7162.3936023290216</c:v>
+                  <c:v>6426.5848606689906</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7039.4363399822614</c:v>
+                  <c:v>6316.2592733611318</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6919.6183352181533</c:v>
+                  <c:v>6208.7504406711514</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6802.8336247343677</c:v>
+                  <c:v>6103.9632851441702</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6688.9806786809768</c:v>
+                  <c:v>6001.8067073192151</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6577.9621799167589</c:v>
+                  <c:v>5902.1933876630137</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6469.6848159826059</c:v>
+                  <c:v>5805.0395999144475</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6364.0590829616576</c:v>
+                  <c:v>5710.2650350945578</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6260.9991004561643</c:v>
+                  <c:v>5617.7926354912688</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6160.4224369667863</c:v>
+                  <c:v>5527.5484379778482</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6062.2499450112846</c:v>
+                  <c:v>5439.4614260702356</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5966.4056053666736</c:v>
+                  <c:v>5353.4633901705347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2254,8 +2359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC6F123-32E7-44A1-9243-3BCDE965A118}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>915</v>
+        <v>821</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -2331,7 +2436,7 @@
       </c>
       <c r="E7" s="9">
         <f>MAX(Calcs!F12:F26)</f>
-        <v>7551.2320942921951</v>
+        <v>6775.477103184583</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2362,7 +2467,7 @@
       </c>
       <c r="E10" s="9">
         <f>E7*B9</f>
-        <v>15102.46418858439</v>
+        <v>13550.954206369166</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2473,7 +2578,7 @@
       </c>
       <c r="C6">
         <f>'Inputs + Answers'!B5*('Inputs + Answers'!B7 ^ 2)</f>
-        <v>8235</v>
+        <v>7389</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,7 +2602,7 @@
       </c>
       <c r="C8">
         <f>(('Inputs + Answers'!$B$7 ^ 2) * ('Inputs + Answers'!$E$5 ^ 2) * ('Inputs + Answers'!$B$5 - 'Inputs + Answers'!$B$6) )</f>
-        <v>93801.796875</v>
+        <v>84165.328125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2553,19 +2658,19 @@
       </c>
       <c r="C12" s="2">
         <f>( $C$6 - $C$7 - ($C$8/(B12^2))) / ($C$9)</f>
-        <v>-915</v>
+        <v>-821</v>
       </c>
       <c r="D12" s="2">
         <f>( $C$6 - $C$7 + ($C$8/(B12^2))) / ($C$9)</f>
-        <v>7804.411764705882</v>
+        <v>7002.6470588235297</v>
       </c>
       <c r="E12" s="2">
         <f>$C$6 / $C$9</f>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F12" s="8">
         <f>SQRT((0.5*((D12-E12)^2 + (E12-C12)^2 + (C12-D12)^2)))</f>
-        <v>7551.2320942921951</v>
+        <v>6775.477103184583</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2578,19 +2683,19 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ref="C13:C26" si="0">( $C$6 - $C$7 - ($C$8/(B13^2))) / ($C$9)</f>
-        <v>-838.17849294937537</v>
+        <v>-752.07053848244539</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ref="D13:D26" si="1">( $C$6 - $C$7 + ($C$8/(B13^2))) / ($C$9)</f>
-        <v>7727.5902576552571</v>
+        <v>6933.7175973059757</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" ref="E13:E26" si="2">$C$6 / $C$9</f>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F13" s="8">
         <f t="shared" ref="F13:F26" si="3">SQRT((0.5*((D13-E13)^2 + (E13-C13)^2 + (C13-D13)^2)))</f>
-        <v>7418.1733409665039</v>
+        <v>6656.0877736978155</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2603,19 +2708,19 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>-763.36972462115091</v>
+        <v>-684.94704252892336</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>7652.7814893270324</v>
+        <v>6866.5941013524525</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" si="3"/>
-        <v>7288.6007533703687</v>
+        <v>6539.8264683246707</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,19 +2733,19 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>-690.50399199377262</v>
+        <v>-619.56696986545069</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>7579.9157566996546</v>
+        <v>6801.2140286889799</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="3"/>
-        <v>7162.3936023290216</v>
+        <v>6426.5848606689906</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2653,19 +2758,19 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>-619.51458347905157</v>
+        <v>-555.87046233475519</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>7508.9263481849339</v>
+        <v>6737.5175211582846</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="3"/>
-        <v>7039.4363399822614</v>
+        <v>6316.2592733611318</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2678,19 +2783,19 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>-550.33762617472996</v>
+        <v>-493.80020884093233</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>7439.7493908806118</v>
+        <v>6675.4472676644618</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="3"/>
-        <v>6919.6183352181533</v>
+        <v>6208.7504406711514</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2703,19 +2808,19 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>-482.91194213968339</v>
+        <v>-433.30131638981402</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>7372.3237068455655</v>
+        <v>6614.9483752133438</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="3"/>
-        <v>6802.8336247343677</v>
+        <v>6103.9632851441702</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2728,19 +2833,19 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>-417.17891308772636</v>
+        <v>-374.32118868308595</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>7306.5906777936098</v>
+        <v>6555.9682475066156</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" si="3"/>
-        <v>6688.9806786809768</v>
+        <v>6001.8067073192151</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2753,19 +2858,19 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>-353.08235294117634</v>
+        <v>-316.80941176470566</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>7242.4941176470593</v>
+        <v>6498.4564705882349</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" si="3"/>
-        <v>6577.9621799167589</v>
+        <v>5902.1933876630137</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2778,19 +2883,19 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>-290.56838772665054</v>
+        <v>-260.71764625527885</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>7179.980152432533</v>
+        <v>6442.3647050788086</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F21" s="8">
         <f t="shared" si="3"/>
-        <v>6469.6848159826059</v>
+        <v>5805.0395999144475</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2803,19 +2908,19 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>-229.58534233365435</v>
+        <v>-205.99952574418646</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>7118.9971070395377</v>
+        <v>6387.6465845677158</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" si="3"/>
-        <v>6364.0590829616576</v>
+        <v>5710.2650350945578</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2828,19 +2933,19 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" si="0"/>
-        <v>-170.08363369143007</v>
+        <v>-152.61056094061664</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>7059.4953983973128</v>
+        <v>6334.2576197641456</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="3"/>
-        <v>6260.9991004561643</v>
+        <v>5617.7926354912688</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2853,19 +2958,19 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>-112.01566995164301</v>
+        <v>-100.50804921344123</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>7001.4274346575257</v>
+        <v>6282.1551080369709</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" si="3"/>
-        <v>6160.4224369667863</v>
+        <v>5527.5484379778482</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2878,19 +2983,19 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>-55.335755294118094</v>
+        <v>-49.650989176470745</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>6944.7475200000008</v>
+        <v>6231.2980480000006</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" si="3"/>
-        <v>6062.2499450112846</v>
+        <v>5439.4614260702356</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2907,15 +3012,15 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>6889.411764705882</v>
+        <v>6181.6470588235297</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>3444.705882352941</v>
+        <v>3090.8235294117649</v>
       </c>
       <c r="F26" s="8">
         <f t="shared" si="3"/>
-        <v>5966.4056053666736</v>
+        <v>5353.4633901705347</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2930,4 +3035,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EE0F68-5A2B-4B82-BFC6-02B19F6DD309}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <f>Calcs!E12</f>
+        <v>3090.8235294117649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <f>'Inputs + Answers'!B7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="21">
+        <f>3/8</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+    </row>
+    <row r="12" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <f>(4*PI()*(B7^2))/2</f>
+        <v>56.548667764616276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <f>B6/B13</f>
+        <v>54.657760325624508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <f>B14/B9</f>
+        <v>6.8322200407030635</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <f>B15/(PI()*(B10^2)/4)</f>
+        <v>61.859930553992704</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated flight_sim matlab programs
</commit_message>
<xml_diff>
--- a/Thick Walled PV Basic Stress Calc.xlsx
+++ b/Thick Walled PV Basic Stress Calc.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD Documents\Rocketry\Propulsion Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danzanko/Documents/GitHub/Propulsion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{27AE3C5D-3511-4AB5-BAC9-F1852AB5542B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616B38B0-8BA5-F046-90D8-2BC38435C4CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{838B0196-D158-479E-A7C6-911A07F6EFB7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{838B0196-D158-479E-A7C6-911A07F6EFB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs + Answers" sheetId="1" r:id="rId1"/>
     <sheet name="Calcs" sheetId="2" r:id="rId2"/>
     <sheet name="Bolt Calcs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Dan Zanko - 7/22/2018</t>
   </si>
@@ -135,12 +135,6 @@
   </si>
   <si>
     <t>Maximum vM-Equivalent Stress (psi) =</t>
-  </si>
-  <si>
-    <t>Factor of Safety</t>
-  </si>
-  <si>
-    <t>Max vM-Equiv w/ Factor of Safety (psi)</t>
   </si>
   <si>
     <r>
@@ -310,6 +304,9 @@
   </si>
   <si>
     <t>Tensile Stress on Each Bolt (psi)</t>
+  </si>
+  <si>
+    <t>Factor of Safety (multiplying the pressure)</t>
   </si>
 </sst>
 </file>
@@ -458,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -483,6 +480,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,12 +504,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,49 +581,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0267857142857144</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0535714285714284</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0803571428571428</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1071428571428572</c:v>
+                  <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1339285714285716</c:v>
+                  <c:v>0.19750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1607142857142856</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1875</c:v>
+                  <c:v>0.20250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2142857142857144</c:v>
+                  <c:v>0.20499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2410714285714284</c:v>
+                  <c:v>0.20749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2678571428571428</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2946428571428572</c:v>
+                  <c:v>0.21249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.3214285714285716</c:v>
+                  <c:v>0.215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3482142857142856</c:v>
+                  <c:v>0.2175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.375</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -635,49 +635,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7002.6470588235297</c:v>
+                  <c:v>9571.093474426807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6933.7175973059757</c:v>
+                  <c:v>9422.5822808543999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6866.5941013524525</c:v>
+                  <c:v>9279.8947173000724</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6801.2140286889799</c:v>
+                  <c:v>9142.7302307166265</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6737.5175211582846</c:v>
+                  <c:v>9010.8074099584064</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6675.4472676644618</c:v>
+                  <c:v>8883.8625412481088</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6614.9483752133438</c:v>
+                  <c:v>8761.6482892416225</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6555.9682475066156</c:v>
+                  <c:v>8643.9324913637756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6498.4564705882349</c:v>
+                  <c:v>8530.4970544324096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6442.3647050788086</c:v>
+                  <c:v>8421.1369437717731</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6387.6465845677158</c:v>
+                  <c:v>8315.6592560598619</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6334.2576197641456</c:v>
+                  <c:v>8213.8823680757705</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6282.1551080369709</c:v>
+                  <c:v>8115.6351543281417</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6231.2980480000006</c:v>
+                  <c:v>8020.7562672676513</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6181.6470588235297</c:v>
+                  <c:v>7929.093474426807</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,49 +726,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0267857142857144</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0535714285714284</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0803571428571428</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1071428571428572</c:v>
+                  <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1339285714285716</c:v>
+                  <c:v>0.19750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1607142857142856</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1875</c:v>
+                  <c:v>0.20250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2142857142857144</c:v>
+                  <c:v>0.20499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2410714285714284</c:v>
+                  <c:v>0.20749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2678571428571428</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2946428571428572</c:v>
+                  <c:v>0.21249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.3214285714285716</c:v>
+                  <c:v>0.215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3482142857142856</c:v>
+                  <c:v>0.2175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.375</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,46 +780,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-821</c:v>
+                  <c:v>-1641.9999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-752.07053848244539</c:v>
+                  <c:v>-1493.488806427592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-684.94704252892336</c:v>
+                  <c:v>-1350.801242873265</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-619.56696986545069</c:v>
+                  <c:v>-1213.6367562898179</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-555.87046233475519</c:v>
+                  <c:v>-1081.713935531599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-493.80020884093233</c:v>
+                  <c:v>-954.76906682130118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-433.30131638981402</c:v>
+                  <c:v>-832.55481481481388</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-374.32118868308595</c:v>
+                  <c:v>-714.83901693696816</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-316.80941176470566</c:v>
+                  <c:v>-601.4035800056032</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-260.71764625527885</c:v>
+                  <c:v>-492.04346934496454</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-205.99952574418646</c:v>
+                  <c:v>-386.5657816330534</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-152.61056094061664</c:v>
+                  <c:v>-284.7888936489631</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-100.50804921344123</c:v>
+                  <c:v>-186.54167990133428</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-49.650989176470745</c:v>
+                  <c:v>-91.662792840843792</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -871,49 +871,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0267857142857144</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0535714285714284</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0803571428571428</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1071428571428572</c:v>
+                  <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1339285714285716</c:v>
+                  <c:v>0.19750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1607142857142856</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1875</c:v>
+                  <c:v>0.20250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2142857142857144</c:v>
+                  <c:v>0.20499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2410714285714284</c:v>
+                  <c:v>0.20749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2678571428571428</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2946428571428572</c:v>
+                  <c:v>0.21249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.3214285714285716</c:v>
+                  <c:v>0.215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3482142857142856</c:v>
+                  <c:v>0.2175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.375</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -925,49 +925,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3090.8235294117649</c:v>
+                  <c:v>3964.5467372134035</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1022,49 +1022,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0267857142857144</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0535714285714284</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0803571428571428</c:v>
+                  <c:v>0.1925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1071428571428572</c:v>
+                  <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1339285714285716</c:v>
+                  <c:v>0.19750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1607142857142856</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1875</c:v>
+                  <c:v>0.20250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2142857142857144</c:v>
+                  <c:v>0.20499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2410714285714284</c:v>
+                  <c:v>0.20749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2678571428571428</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2946428571428572</c:v>
+                  <c:v>0.21249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.3214285714285716</c:v>
+                  <c:v>0.215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3482142857142856</c:v>
+                  <c:v>0.2175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.375</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,49 +1076,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>6775.477103184583</c:v>
+                  <c:v>9710.8238038631298</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6656.0877736978155</c:v>
+                  <c:v>9453.5948711030233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6539.8264683246707</c:v>
+                  <c:v>9206.4527614187155</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6426.5848606689906</c:v>
+                  <c:v>8968.8769016620863</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6316.2592733611318</c:v>
+                  <c:v>8740.3798734310476</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6208.7504406711514</c:v>
+                  <c:v>8520.5049110646523</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6103.9632851441702</c:v>
+                  <c:v>8308.8236171803892</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6001.8067073192151</c:v>
+                  <c:v>8104.9338744024517</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5902.1933876630137</c:v>
+                  <c:v>7908.4579342585512</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5805.0395999144475</c:v>
+                  <c:v>7719.040666272972</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5710.2650350945578</c:v>
+                  <c:v>7536.3479520910587</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5617.7926354912688</c:v>
+                  <c:v>7360.0652110663677</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5527.5484379778482</c:v>
+                  <c:v>7189.8960451533949</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5439.4614260702356</c:v>
+                  <c:v>7025.5609921990354</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5353.4633901705347</c:v>
+                  <c:v>6866.7963778350331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2359,49 +2359,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC6F123-32E7-44A1-9243-3BCDE965A118}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="D4" s="14" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2413,10 +2413,10 @@
       </c>
       <c r="E5" s="2">
         <f>B7+B8</f>
-        <v>3.375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -2424,27 +2424,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>0.185</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="9">
         <f>MAX(Calcs!F12:F26)</f>
-        <v>6775.477103184583</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9710.8238038631298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="11">
-        <v>0.375</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>33</v>
@@ -2453,48 +2453,43 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="9">
-        <f>E7*B9</f>
-        <v>13550.954206369166</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="9" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="17" spans="4:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2515,44 +2510,44 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="17"/>
+      <c r="C1" s="21"/>
       <c r="D1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="21"/>
       <c r="D2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2563,13 +2558,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -2577,11 +2572,11 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <f>'Inputs + Answers'!B5*('Inputs + Answers'!B7 ^ 2)</f>
-        <v>7389</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <f>(2*'Inputs + Answers'!B5)*('Inputs + Answers'!B7 ^ 2)</f>
+        <v>56.197449999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -2593,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2601,11 +2596,11 @@
         <v>27</v>
       </c>
       <c r="C8">
-        <f>(('Inputs + Answers'!$B$7 ^ 2) * ('Inputs + Answers'!$E$5 ^ 2) * ('Inputs + Answers'!$B$5 - 'Inputs + Answers'!$B$6) )</f>
-        <v>84165.328125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <f>(('Inputs + Answers'!$B$7 ^ 2) * ('Inputs + Answers'!$E$5 ^ 2) * (2*('Inputs + Answers'!$B$5 - 'Inputs + Answers'!$B$6) ))</f>
+        <v>2.7199565799999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2614,10 +2609,10 @@
       </c>
       <c r="C9">
         <f>('Inputs + Answers'!$E$5^2)-('Inputs + Answers'!$B$7^2)</f>
-        <v>2.390625</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.4175E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
@@ -2628,7 +2623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>14</v>
       </c>
@@ -2648,363 +2643,363 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12" s="2">
         <f>'Inputs + Answers'!$B$7 + (A12-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3</v>
+        <v>0.185</v>
       </c>
       <c r="C12" s="2">
         <f>( $C$6 - $C$7 - ($C$8/(B12^2))) / ($C$9)</f>
-        <v>-821</v>
+        <v>-1641.9999999999998</v>
       </c>
       <c r="D12" s="2">
         <f>( $C$6 - $C$7 + ($C$8/(B12^2))) / ($C$9)</f>
-        <v>7002.6470588235297</v>
+        <v>9571.093474426807</v>
       </c>
       <c r="E12" s="2">
         <f>$C$6 / $C$9</f>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F12" s="8">
         <f>SQRT((0.5*((D12-E12)^2 + (E12-C12)^2 + (C12-D12)^2)))</f>
-        <v>6775.477103184583</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9710.8238038631298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13" s="2">
         <f>'Inputs + Answers'!$B$7 + (A13-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.0267857142857144</v>
+        <v>0.1875</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" ref="C13:C26" si="0">( $C$6 - $C$7 - ($C$8/(B13^2))) / ($C$9)</f>
-        <v>-752.07053848244539</v>
+        <v>-1493.488806427592</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ref="D13:D26" si="1">( $C$6 - $C$7 + ($C$8/(B13^2))) / ($C$9)</f>
-        <v>6933.7175973059757</v>
+        <v>9422.5822808543999</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" ref="E13:E26" si="2">$C$6 / $C$9</f>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F13" s="8">
         <f t="shared" ref="F13:F26" si="3">SQRT((0.5*((D13-E13)^2 + (E13-C13)^2 + (C13-D13)^2)))</f>
-        <v>6656.0877736978155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9453.5948711030233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>3</v>
       </c>
       <c r="B14" s="2">
         <f>'Inputs + Answers'!$B$7 + (A14-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.0535714285714284</v>
+        <v>0.19</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>-684.94704252892336</v>
+        <v>-1350.801242873265</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>6866.5941013524525</v>
+        <v>9279.8947173000724</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" si="3"/>
-        <v>6539.8264683246707</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9206.4527614187155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>4</v>
       </c>
       <c r="B15" s="2">
         <f>'Inputs + Answers'!$B$7 + (A15-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.0803571428571428</v>
+        <v>0.1925</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>-619.56696986545069</v>
+        <v>-1213.6367562898179</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>6801.2140286889799</v>
+        <v>9142.7302307166265</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="3"/>
-        <v>6426.5848606689906</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8968.8769016620863</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>5</v>
       </c>
       <c r="B16" s="2">
         <f>'Inputs + Answers'!$B$7 + (A16-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.1071428571428572</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>-555.87046233475519</v>
+        <v>-1081.713935531599</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>6737.5175211582846</v>
+        <v>9010.8074099584064</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="3"/>
-        <v>6316.2592733611318</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8740.3798734310476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>6</v>
       </c>
       <c r="B17" s="2">
         <f>'Inputs + Answers'!$B$7 + (A17-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.1339285714285716</v>
+        <v>0.19750000000000001</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>-493.80020884093233</v>
+        <v>-954.76906682130118</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>6675.4472676644618</v>
+        <v>8883.8625412481088</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="3"/>
-        <v>6208.7504406711514</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8520.5049110646523</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>7</v>
       </c>
       <c r="B18" s="2">
         <f>'Inputs + Answers'!$B$7 + (A18-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.1607142857142856</v>
+        <v>0.2</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>-433.30131638981402</v>
+        <v>-832.55481481481388</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>6614.9483752133438</v>
+        <v>8761.6482892416225</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="3"/>
-        <v>6103.9632851441702</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8308.8236171803892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>8</v>
       </c>
       <c r="B19" s="2">
         <f>'Inputs + Answers'!$B$7 + (A19-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.1875</v>
+        <v>0.20250000000000001</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>-374.32118868308595</v>
+        <v>-714.83901693696816</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>6555.9682475066156</v>
+        <v>8643.9324913637756</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" si="3"/>
-        <v>6001.8067073192151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8104.9338744024517</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>9</v>
       </c>
       <c r="B20" s="2">
         <f>'Inputs + Answers'!$B$7 + (A20-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.2142857142857144</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>-316.80941176470566</v>
+        <v>-601.4035800056032</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>6498.4564705882349</v>
+        <v>8530.4970544324096</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" si="3"/>
-        <v>5902.1933876630137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7908.4579342585512</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>10</v>
       </c>
       <c r="B21" s="2">
         <f>'Inputs + Answers'!$B$7 + (A21-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.2410714285714284</v>
+        <v>0.20749999999999999</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>-260.71764625527885</v>
+        <v>-492.04346934496454</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>6442.3647050788086</v>
+        <v>8421.1369437717731</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F21" s="8">
         <f t="shared" si="3"/>
-        <v>5805.0395999144475</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7719.040666272972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>11</v>
       </c>
       <c r="B22" s="2">
         <f>'Inputs + Answers'!$B$7 + (A22-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.2678571428571428</v>
+        <v>0.21</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>-205.99952574418646</v>
+        <v>-386.5657816330534</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>6387.6465845677158</v>
+        <v>8315.6592560598619</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" si="3"/>
-        <v>5710.2650350945578</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7536.3479520910587</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>12</v>
       </c>
       <c r="B23" s="2">
         <f>'Inputs + Answers'!$B$7 + (A23-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.2946428571428572</v>
+        <v>0.21249999999999999</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="0"/>
-        <v>-152.61056094061664</v>
+        <v>-284.7888936489631</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>6334.2576197641456</v>
+        <v>8213.8823680757705</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="3"/>
-        <v>5617.7926354912688</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7360.0652110663677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>13</v>
       </c>
       <c r="B24" s="2">
         <f>'Inputs + Answers'!$B$7 + (A24-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.3214285714285716</v>
+        <v>0.215</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>-100.50804921344123</v>
+        <v>-186.54167990133428</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>6282.1551080369709</v>
+        <v>8115.6351543281417</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" si="3"/>
-        <v>5527.5484379778482</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7189.8960451533949</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>14</v>
       </c>
       <c r="B25" s="2">
         <f>'Inputs + Answers'!$B$7 + (A25-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.3482142857142856</v>
+        <v>0.2175</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>-49.650989176470745</v>
+        <v>-91.662792840843792</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>6231.2980480000006</v>
+        <v>8020.7562672676513</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" si="3"/>
-        <v>5439.4614260702356</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7025.5609921990354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>15</v>
       </c>
       <c r="B26" s="2">
         <f>'Inputs + Answers'!$B$7 + (A26-1)*('Inputs + Answers'!$E$5-'Inputs + Answers'!$B$7)/Calcs!$A$11</f>
-        <v>3.375</v>
+        <v>0.22</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="0"/>
@@ -3012,18 +3007,18 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>6181.6470588235297</v>
+        <v>7929.093474426807</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>3090.8235294117649</v>
+        <v>3964.5467372134035</v>
       </c>
       <c r="F26" s="8">
         <f t="shared" si="3"/>
-        <v>5353.4633901705347</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6866.7963778350331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
     </row>
   </sheetData>
@@ -3041,115 +3036,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EE0F68-5A2B-4B82-BFC6-02B19F6DD309}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="B6">
         <f>Calcs!E12</f>
-        <v>3090.8235294117649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>47</v>
+        <v>3964.5467372134035</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B7">
         <f>'Inputs + Answers'!B7</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>52</v>
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="21">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="15">
         <f>3/8</f>
         <v>0.375</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-    </row>
-    <row r="12" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+    </row>
+    <row r="12" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>48</v>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="B13">
         <f>(4*PI()*(B7^2))/2</f>
-        <v>56.548667764616276</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>51</v>
+        <v>0.21504201713822133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="B14">
         <f>B6/B13</f>
-        <v>54.657760325624508</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>54</v>
+        <v>18436.149316182866</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="B15">
         <f>B14/B9</f>
-        <v>6.8322200407030635</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>55</v>
+        <v>2304.5186645228582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B16">
         <f>B15/(PI()*(B10^2)/4)</f>
-        <v>61.859930553992704</v>
+        <v>20865.452766227692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>